<commit_message>
Organizing, updating, final report
</commit_message>
<xml_diff>
--- a/SMTO_2019/Location_Choice/Subset/Subset_Results.xlsx
+++ b/SMTO_2019/Location_Choice/Subset/Subset_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\R_Logit_Models\SMTO_2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\SMTO_2019\Location_Choice\Subset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94DB16D6-0733-41FB-97B0-BC24D6460FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EA9C35-114A-4A81-B5DC-615292CFD042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{C76CCB26-B987-4C6F-9AA7-27F3459D6F4C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{C76CCB26-B987-4C6F-9AA7-27F3459D6F4C}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Prec</t>
   </si>
@@ -107,15 +107,40 @@
   </si>
   <si>
     <t>Joint</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Parameter/Metric</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>log(Total)</t>
+  </si>
+  <si>
+    <t>IsClosest</t>
+  </si>
+  <si>
+    <t>Mean log loss</t>
+  </si>
+  <si>
+    <t>Sample size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -157,21 +182,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="8" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -182,6 +240,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{264D5E44-BD53-4A22-A000-D1A7C67130D2}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:D7" xr:uid="{0D28A141-495A-4307-BC73-3EED0A672ACE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E40AB45D-9A60-4644-B9C1-A0B30C34FCC6}" name="Parameter/Metric"/>
+    <tableColumn id="2" xr3:uid="{D6AE2FF8-9A3C-4F8C-9F12-0E29CE56EF0C}" name="2015" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D9EF65CE-ABA7-46DD-9BD6-59C54104C08B}" name="2019" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C8B3B495-65E8-4E4E-82A5-681BDFD27429}" name="Joint" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA839C3-0A9F-47FC-A760-E203CB9EA243}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1084,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2172E46A-DEAB-449C-A552-837581532626}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1095,18 +1166,21 @@
     <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>2015</v>
-      </c>
-      <c r="C1">
-        <v>2019</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1120,7 +1194,7 @@
         <v>-9.2747300000000005E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1134,7 +1208,7 @@
         <v>0.86604970000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1148,7 +1222,7 @@
         <v>1.0258425</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1162,7 +1236,7 @@
         <v>3.7495800000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1176,7 +1250,7 @@
         <v>0.42934119999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1188,6 +1262,231 @@
       </c>
       <c r="D7" s="3">
         <v>0.3301463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>2015</v>
+      </c>
+      <c r="E10">
+        <v>2019</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
+        <v>-0.10885499999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2.3860999999999999E-3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-8.9210499999999998E-2</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1.9517E-3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-9.2747300000000005E-2</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1.4109999999999999E-3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.89906870000000005</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.2079599999999999E-2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.84043650000000003</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1.31503E-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.86604970000000003</v>
+      </c>
+      <c r="I12" s="6">
+        <v>8.8502000000000008E-3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.90420449999999997</v>
+      </c>
+      <c r="C13" s="6">
+        <v>4.1341799999999998E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.0643768</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4.7429699999999998E-2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.0258425</v>
+      </c>
+      <c r="I13" s="6">
+        <v>3.1608799999999999E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6">
+        <v>5.0717600000000002E-2</v>
+      </c>
+      <c r="C14" s="6">
+        <v>2.7352000000000001E-3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3.6976500000000002E-2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>2.7777000000000001E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="6">
+        <v>3.7495800000000003E-2</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1.7742000000000001E-3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="6">
+        <v>0.46221849999999998</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6">
+        <v>0.38403219999999999</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6">
+        <v>0.42934119999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="6">
+        <v>0.34793089999999999</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6">
+        <v>0.30691279999999999</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6">
+        <v>0.3301463</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B18" s="2">
+        <v>-19307.09</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
+        <v>-15560.44</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <v>-34801.32</v>
+      </c>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
+        <f>B18/B20</f>
+        <v>-1.333546760602293</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <f>E18/E20</f>
+        <v>-1.4214341828811548</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <f>H18/H20</f>
+        <v>-1.3687834808259587</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="7">
+        <v>14478</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7">
+        <v>10947</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7">
+        <v>25425</v>
       </c>
     </row>
   </sheetData>
@@ -1216,5 +1515,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>